<commit_message>
Created 6 test cases to on the project
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3bb12600baa2005/Documents/TRABAJO/TechMahindra/bootcamp/SampleProject_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="11_F25DC773A252ABDACC104880295A4B9C5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28F9029-E709-44DE-9B36-1961486D539A}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="11_F25DC773A252ABDACC104880295A4B9C5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CFE355-5C5E-405A-9AC4-50410CC22866}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,21 +205,9 @@
     <t xml:space="preserve">User can navigate through the carrousel </t>
   </si>
   <si>
-    <t>As a user I want to navigate through all categories menu</t>
-  </si>
-  <si>
-    <t>User can navigate through the all categories menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can navigate through "All" category menu </t>
-  </si>
-  <si>
     <t>User can navigate through the "Phones" category menu</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Load the website.                  2. Log in on the website.                            3. Click on categories Button.                                                                 4. Check that appear elements of all categories                                                            </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Load the website.                  2. Log in on the website.                            3. Click on Phones Button.                                                                   4. Check that appear elements of all categories                                                            </t>
   </si>
   <si>
@@ -250,9 +238,6 @@
     <t>Carrousel Test</t>
   </si>
   <si>
-    <t>Category All</t>
-  </si>
-  <si>
     <t>Category Phones</t>
   </si>
   <si>
@@ -320,6 +305,21 @@
   </si>
   <si>
     <t xml:space="preserve">Buying Items </t>
+  </si>
+  <si>
+    <t>Contact Form</t>
+  </si>
+  <si>
+    <t>User can use contact form to get support</t>
+  </si>
+  <si>
+    <t>As a user I want to use the contact form to get support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Load the website.                  2. Log in on the website.                            3. Click on contact.                                                                 4. Fill the form.                           5. Validate the success message                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can use contact form </t>
   </si>
 </sst>
 </file>
@@ -1080,69 +1080,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1151,6 +1088,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1158,6 +1116,48 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1826,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1857,15 +1857,15 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="76" t="s">
+      <c r="H1" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="6"/>
@@ -1892,13 +1892,13 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="7"/>
@@ -1925,13 +1925,13 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="7"/>
@@ -1961,13 +1961,13 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="100"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1993,19 +1993,19 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="82">
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="96">
         <f>COUNTA($I$25:$I$1000)</f>
         <v>10</v>
       </c>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="84"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="91"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
@@ -2031,19 +2031,19 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="82">
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="96">
         <f>COUNTIF($Z$25:$Z$1000,"Ok")+COUNTIF($Z$25:$Z$1000,"FALLO")</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="84"/>
+        <v>5</v>
+      </c>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="91"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -2068,19 +2068,19 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="82">
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="96">
         <f>COUNTIF($Z$25:$Z$1000,"Ok")</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="84"/>
+        <v>5</v>
+      </c>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="91"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
@@ -2105,19 +2105,19 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="82">
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="96">
         <f>COUNTIF($Z$25:$Z$1000,"Fallo")</f>
         <v>0</v>
       </c>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="84"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="91"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -2142,19 +2142,19 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="85" t="s">
+      <c r="H9" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="86"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="90">
+      <c r="I9" s="82"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="89">
         <f>SUM(K5-K6)</f>
-        <v>10</v>
-      </c>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="84"/>
+        <v>5</v>
+      </c>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="91"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -2179,30 +2179,30 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="85" t="s">
+      <c r="H10" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="91">
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="92">
         <f>($K$17+$L$17+$M$17+N$17+O$17)/($K$5)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="93"/>
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="94"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
-      <c r="V10" s="94"/>
-      <c r="W10" s="94"/>
-      <c r="X10" s="94"/>
-      <c r="Y10" s="94"/>
-      <c r="Z10" s="94"/>
+      <c r="V10" s="95"/>
+      <c r="W10" s="95"/>
+      <c r="X10" s="95"/>
+      <c r="Y10" s="95"/>
+      <c r="Z10" s="95"/>
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="12" t="s">
@@ -2218,19 +2218,19 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="85" t="s">
+      <c r="H11" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="91">
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="92">
         <f>$K$6/($K$5)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="93"/>
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="94"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
@@ -2257,19 +2257,19 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="91">
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="92">
         <f>$K$7/($K$5)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="93"/>
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="93"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="94"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
@@ -2302,14 +2302,14 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="88"/>
-      <c r="R13" s="88"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="88"/>
-      <c r="U13" s="88"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
       <c r="V13" s="87"/>
       <c r="W13" s="87"/>
       <c r="X13" s="87"/>
@@ -2335,14 +2335,14 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="88"/>
-      <c r="R14" s="88"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
+      <c r="U14" s="78"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
@@ -2405,11 +2405,11 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="80" t="s">
+      <c r="H16" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="31">
         <f>K5</f>
         <v>10</v>
@@ -2455,14 +2455,14 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="85" t="s">
+      <c r="H17" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
       <c r="K17" s="31">
         <f>SUM(K18,K19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L17" s="31">
         <f>SUM(L18,L19)</f>
@@ -2507,14 +2507,14 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="85" t="s">
+      <c r="H18" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
       <c r="K18" s="31">
-        <f>COUNTIF($K$25:$K$1000,"Exitoso")</f>
-        <v>0</v>
+        <f>COUNTIF($K$25:$K$1000,"Successful")</f>
+        <v>5</v>
       </c>
       <c r="L18" s="31">
         <f>COUNTIF($N$25:$N$1000,"Exitoso")</f>
@@ -2559,13 +2559,13 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="85" t="s">
+      <c r="H19" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
       <c r="K19" s="31">
-        <f>COUNTIF($K$25:$K$1000,"Fallido")</f>
+        <f>COUNTIF($K$25:$K$1000,"Failed")</f>
         <v>0</v>
       </c>
       <c r="L19" s="31">
@@ -2611,14 +2611,14 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="30"/>
-      <c r="H20" s="85" t="s">
+      <c r="H20" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
       <c r="K20" s="32">
         <f>$K$17/($K$16)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L20" s="32">
         <f>$L$17/($L$16)</f>
@@ -2661,14 +2661,14 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="30"/>
-      <c r="H21" s="95" t="s">
+      <c r="H21" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="96"/>
-      <c r="J21" s="96"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
       <c r="K21" s="32">
         <f>$K$18/($K$16)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L21" s="32">
         <f>$L$18/($L$16)</f>
@@ -2776,10 +2776,10 @@
       <c r="B24" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="100"/>
+      <c r="D24" s="86"/>
       <c r="E24" s="41" t="s">
         <v>8</v>
       </c>
@@ -2857,10 +2857,10 @@
     <row r="25" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="46"/>
       <c r="B25" s="47"/>
-      <c r="C25" s="97" t="s">
+      <c r="C25" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="98"/>
+      <c r="D25" s="77"/>
       <c r="E25" s="48" t="s">
         <v>34</v>
       </c>
@@ -2877,10 +2877,10 @@
         <v>36</v>
       </c>
       <c r="J25" s="53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L25" s="55"/>
       <c r="M25" s="56"/>
@@ -2898,7 +2898,7 @@
       <c r="Y25" s="53"/>
       <c r="Z25" s="57" t="str">
         <f>IF(W25="Successful","OK",IF(W25="Failed","FAILED",IF(W25="Pending","PENDING",IF(T25="Succesful","OK",IF(T25="Failed","FAILED",IF(T25="Pending","PENDING",IF(Q25="Successful","OK",IF(Q25="Failed","FAILED",IF(Q25="Pending","PENDING",IF(N25="Successful","OK",IF(N25="Failed","FAILED",IF(N25="Pending","PENDING",IF(K25="Successful","OK",IF(K25="Failed","FAILED",IF(K25="Pending","PENDING")))))))))))))))</f>
-        <v>PENDING</v>
+        <v>OK</v>
       </c>
       <c r="AA25" s="53"/>
       <c r="AB25" s="58"/>
@@ -2909,10 +2909,10 @@
     <row r="26" spans="1:31" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="46"/>
       <c r="B26" s="47"/>
-      <c r="C26" s="97" t="s">
+      <c r="C26" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="98"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="59" t="s">
         <v>44</v>
       </c>
@@ -2929,10 +2929,10 @@
         <v>47</v>
       </c>
       <c r="J26" s="53" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K26" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L26" s="55"/>
       <c r="M26" s="56"/>
@@ -2948,9 +2948,9 @@
       <c r="W26" s="54"/>
       <c r="X26" s="53"/>
       <c r="Y26" s="53"/>
-      <c r="Z26" s="57" t="b">
-        <f t="shared" ref="Z26:Z76" si="0">IF(W26="Exitoso","OK",IF(W26="Fallido","FALLO",IF(W26="Pendiente","PENDIENTE",IF(T26="Exitoso","OK",IF(T26="Fallido","FALLO",IF(T26="Pendiente","PENDIENTE",IF(Q26="Exitoso","OK",IF(Q26="Fallido","FALLO",IF(Q26="Pendiente","PENDIENTE",IF(N26="Exitoso","OK",IF(N26="Fallido","FALLO",IF(N26="Pendiente","PENDIENTE",IF(K26="Exitoso","OK",IF(K26="Fallido","FALLO",IF(K26="Pendiente","PENDIENTE")))))))))))))))</f>
-        <v>0</v>
+      <c r="Z26" s="57" t="str">
+        <f t="shared" ref="Z26:Z37" si="0">IF(W26="Successful","OK",IF(W26="Failed","FAILED",IF(W26="Pending","PENDING",IF(T26="Succesful","OK",IF(T26="Failed","FAILED",IF(T26="Pending","PENDING",IF(Q26="Successful","OK",IF(Q26="Failed","FAILED",IF(Q26="Pending","PENDING",IF(N26="Successful","OK",IF(N26="Failed","FAILED",IF(N26="Pending","PENDING",IF(K26="Successful","OK",IF(K26="Failed","FAILED",IF(K26="Pending","PENDING")))))))))))))))</f>
+        <v>OK</v>
       </c>
       <c r="AA26" s="53"/>
       <c r="AB26" s="58"/>
@@ -2961,10 +2961,10 @@
     <row r="27" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="46"/>
       <c r="B27" s="47"/>
-      <c r="C27" s="97" t="s">
+      <c r="C27" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="77"/>
       <c r="E27" s="59" t="s">
         <v>49</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>52</v>
       </c>
       <c r="J27" s="53" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K27" s="54" t="s">
         <v>41</v>
@@ -3000,9 +3000,9 @@
       <c r="W27" s="54"/>
       <c r="X27" s="53"/>
       <c r="Y27" s="53"/>
-      <c r="Z27" s="57" t="b">
+      <c r="Z27" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>PENDING</v>
       </c>
       <c r="AA27" s="53"/>
       <c r="AB27" s="58"/>
@@ -3010,15 +3010,15 @@
       <c r="AD27" s="58"/>
       <c r="AE27" s="58"/>
     </row>
-    <row r="28" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="46"/>
       <c r="B28" s="47"/>
-      <c r="C28" s="97" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="98"/>
+      <c r="C28" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="77"/>
       <c r="E28" s="62" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="F28" s="60" t="s">
         <v>50</v>
@@ -3027,16 +3027,16 @@
         <v>4</v>
       </c>
       <c r="H28" s="51" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="I28" s="52" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="J28" s="53" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L28" s="65"/>
       <c r="M28" s="56"/>
@@ -3052,9 +3052,9 @@
       <c r="W28" s="54"/>
       <c r="X28" s="53"/>
       <c r="Y28" s="53"/>
-      <c r="Z28" s="57" t="b">
+      <c r="Z28" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>OK</v>
       </c>
       <c r="AA28" s="53"/>
       <c r="AB28" s="58"/>
@@ -3065,12 +3065,12 @@
     <row r="29" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="46"/>
       <c r="B29" s="47"/>
-      <c r="C29" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="98"/>
+      <c r="C29" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="77"/>
       <c r="E29" s="66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F29" s="60" t="s">
         <v>50</v>
@@ -3079,16 +3079,16 @@
         <v>5</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I29" s="52" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J29" s="53" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L29" s="65"/>
       <c r="M29" s="56"/>
@@ -3104,9 +3104,9 @@
       <c r="W29" s="54"/>
       <c r="X29" s="53"/>
       <c r="Y29" s="53"/>
-      <c r="Z29" s="57" t="b">
+      <c r="Z29" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>OK</v>
       </c>
       <c r="AA29" s="53"/>
       <c r="AB29" s="58"/>
@@ -3117,12 +3117,12 @@
     <row r="30" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="46"/>
       <c r="B30" s="47"/>
-      <c r="C30" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="98"/>
+      <c r="C30" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="77"/>
       <c r="E30" s="66" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F30" s="60" t="s">
         <v>50</v>
@@ -3131,16 +3131,16 @@
         <v>6</v>
       </c>
       <c r="H30" s="51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I30" s="52" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J30" s="53" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K30" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L30" s="65"/>
       <c r="M30" s="56"/>
@@ -3156,9 +3156,9 @@
       <c r="W30" s="54"/>
       <c r="X30" s="53"/>
       <c r="Y30" s="53"/>
-      <c r="Z30" s="57" t="b">
+      <c r="Z30" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>OK</v>
       </c>
       <c r="AA30" s="53"/>
       <c r="AB30" s="58"/>
@@ -3169,12 +3169,12 @@
     <row r="31" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
       <c r="B31" s="47"/>
-      <c r="C31" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="98"/>
+      <c r="C31" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="77"/>
       <c r="E31" s="66" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F31" s="60" t="s">
         <v>50</v>
@@ -3183,13 +3183,13 @@
         <v>7</v>
       </c>
       <c r="H31" s="51" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I31" s="52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J31" s="53" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K31" s="54" t="s">
         <v>41</v>
@@ -3208,9 +3208,9 @@
       <c r="W31" s="54"/>
       <c r="X31" s="53"/>
       <c r="Y31" s="53"/>
-      <c r="Z31" s="57" t="b">
+      <c r="Z31" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>PENDING</v>
       </c>
       <c r="AA31" s="53"/>
       <c r="AB31" s="58"/>
@@ -3221,12 +3221,12 @@
     <row r="32" spans="1:31" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="46"/>
       <c r="B32" s="47"/>
-      <c r="C32" s="97" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="98"/>
+      <c r="C32" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="77"/>
       <c r="E32" s="69" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F32" s="60" t="s">
         <v>50</v>
@@ -3235,13 +3235,13 @@
         <v>8</v>
       </c>
       <c r="H32" s="51" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J32" s="53" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K32" s="54" t="s">
         <v>41</v>
@@ -3260,9 +3260,9 @@
       <c r="W32" s="54"/>
       <c r="X32" s="53"/>
       <c r="Y32" s="53"/>
-      <c r="Z32" s="57" t="b">
+      <c r="Z32" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>PENDING</v>
       </c>
       <c r="AA32" s="53"/>
       <c r="AB32" s="58"/>
@@ -3273,27 +3273,27 @@
     <row r="33" spans="1:31" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="46"/>
       <c r="B33" s="47"/>
-      <c r="C33" s="97" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="98"/>
+      <c r="C33" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="77"/>
       <c r="E33" s="69" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F33" s="60" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G33" s="72">
         <v>9</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J33" s="53" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K33" s="54" t="s">
         <v>41</v>
@@ -3312,9 +3312,9 @@
       <c r="W33" s="54"/>
       <c r="X33" s="53"/>
       <c r="Y33" s="53"/>
-      <c r="Z33" s="57" t="b">
+      <c r="Z33" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>PENDING</v>
       </c>
       <c r="AA33" s="53"/>
       <c r="AB33" s="58"/>
@@ -3325,27 +3325,27 @@
     <row r="34" spans="1:31" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="46"/>
       <c r="B34" s="47"/>
-      <c r="C34" s="97" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="98"/>
+      <c r="C34" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="77"/>
       <c r="E34" s="75" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F34" s="60" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G34" s="72">
         <v>10</v>
       </c>
       <c r="H34" s="51" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I34" s="52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J34" s="53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K34" s="54" t="s">
         <v>41</v>
@@ -3364,9 +3364,9 @@
       <c r="W34" s="54"/>
       <c r="X34" s="53"/>
       <c r="Y34" s="53"/>
-      <c r="Z34" s="57" t="b">
+      <c r="Z34" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>PENDING</v>
       </c>
       <c r="AA34" s="53"/>
       <c r="AB34" s="58"/>
@@ -3377,8 +3377,8 @@
     <row r="35" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="46"/>
       <c r="B35" s="47"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="98"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
       <c r="E35" s="69"/>
       <c r="F35" s="74"/>
       <c r="G35" s="72"/>
@@ -3413,8 +3413,8 @@
     <row r="36" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="46"/>
       <c r="B36" s="47"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="98"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
       <c r="E36" s="48"/>
       <c r="F36" s="49"/>
       <c r="G36" s="50"/>
@@ -3449,8 +3449,8 @@
     <row r="37" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="46"/>
       <c r="B37" s="47"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="98"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
       <c r="E37" s="59"/>
       <c r="F37" s="60"/>
       <c r="G37" s="50"/>
@@ -3485,8 +3485,8 @@
     <row r="38" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="46"/>
       <c r="B38" s="47"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="98"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="77"/>
       <c r="E38" s="59"/>
       <c r="F38" s="60"/>
       <c r="G38" s="50"/>
@@ -3509,7 +3509,7 @@
       <c r="X38" s="53"/>
       <c r="Y38" s="53"/>
       <c r="Z38" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Z26:Z76" si="1">IF(W38="Exitoso","OK",IF(W38="Fallido","FALLO",IF(W38="Pendiente","PENDIENTE",IF(T38="Exitoso","OK",IF(T38="Fallido","FALLO",IF(T38="Pendiente","PENDIENTE",IF(Q38="Exitoso","OK",IF(Q38="Fallido","FALLO",IF(Q38="Pendiente","PENDIENTE",IF(N38="Exitoso","OK",IF(N38="Fallido","FALLO",IF(N38="Pendiente","PENDIENTE",IF(K38="Exitoso","OK",IF(K38="Fallido","FALLO",IF(K38="Pendiente","PENDIENTE")))))))))))))))</f>
         <v>0</v>
       </c>
       <c r="AA38" s="53"/>
@@ -3521,8 +3521,8 @@
     <row r="39" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="46"/>
       <c r="B39" s="47"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="98"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="77"/>
       <c r="E39" s="62"/>
       <c r="F39" s="63"/>
       <c r="G39" s="64"/>
@@ -3545,7 +3545,7 @@
       <c r="X39" s="53"/>
       <c r="Y39" s="53"/>
       <c r="Z39" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA39" s="53"/>
@@ -3557,8 +3557,8 @@
     <row r="40" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="46"/>
       <c r="B40" s="47"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="98"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="77"/>
       <c r="E40" s="66"/>
       <c r="F40" s="63"/>
       <c r="G40" s="67"/>
@@ -3581,7 +3581,7 @@
       <c r="X40" s="53"/>
       <c r="Y40" s="53"/>
       <c r="Z40" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA40" s="53"/>
@@ -3593,8 +3593,8 @@
     <row r="41" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="46"/>
       <c r="B41" s="47"/>
-      <c r="C41" s="97"/>
-      <c r="D41" s="98"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="77"/>
       <c r="E41" s="69"/>
       <c r="F41" s="70"/>
       <c r="G41" s="71"/>
@@ -3617,7 +3617,7 @@
       <c r="X41" s="53"/>
       <c r="Y41" s="53"/>
       <c r="Z41" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA41" s="53"/>
@@ -3629,8 +3629,8 @@
     <row r="42" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="46"/>
       <c r="B42" s="47"/>
-      <c r="C42" s="97"/>
-      <c r="D42" s="98"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="77"/>
       <c r="E42" s="69"/>
       <c r="F42" s="70"/>
       <c r="G42" s="72"/>
@@ -3653,7 +3653,7 @@
       <c r="X42" s="53"/>
       <c r="Y42" s="53"/>
       <c r="Z42" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA42" s="53"/>
@@ -3665,8 +3665,8 @@
     <row r="43" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="46"/>
       <c r="B43" s="47"/>
-      <c r="C43" s="97"/>
-      <c r="D43" s="98"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77"/>
       <c r="E43" s="69"/>
       <c r="F43" s="73"/>
       <c r="G43" s="72"/>
@@ -3689,7 +3689,7 @@
       <c r="X43" s="53"/>
       <c r="Y43" s="53"/>
       <c r="Z43" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA43" s="53"/>
@@ -3701,8 +3701,8 @@
     <row r="44" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="46"/>
       <c r="B44" s="47"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="98"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="77"/>
       <c r="E44" s="69"/>
       <c r="F44" s="74"/>
       <c r="G44" s="72"/>
@@ -3725,7 +3725,7 @@
       <c r="X44" s="53"/>
       <c r="Y44" s="53"/>
       <c r="Z44" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA44" s="53"/>
@@ -3737,8 +3737,8 @@
     <row r="45" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="46"/>
       <c r="B45" s="47"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="98"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="77"/>
       <c r="E45" s="75"/>
       <c r="F45" s="74"/>
       <c r="G45" s="72"/>
@@ -3761,7 +3761,7 @@
       <c r="X45" s="53"/>
       <c r="Y45" s="53"/>
       <c r="Z45" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA45" s="53"/>
@@ -3773,8 +3773,8 @@
     <row r="46" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="46"/>
       <c r="B46" s="47"/>
-      <c r="C46" s="97"/>
-      <c r="D46" s="98"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="77"/>
       <c r="E46" s="69"/>
       <c r="F46" s="74"/>
       <c r="G46" s="72"/>
@@ -3797,7 +3797,7 @@
       <c r="X46" s="53"/>
       <c r="Y46" s="53"/>
       <c r="Z46" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA46" s="53"/>
@@ -3809,8 +3809,8 @@
     <row r="47" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="46"/>
       <c r="B47" s="47"/>
-      <c r="C47" s="97"/>
-      <c r="D47" s="98"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="77"/>
       <c r="E47" s="48"/>
       <c r="F47" s="49"/>
       <c r="G47" s="50"/>
@@ -3833,7 +3833,7 @@
       <c r="X47" s="53"/>
       <c r="Y47" s="53"/>
       <c r="Z47" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA47" s="53"/>
@@ -3845,8 +3845,8 @@
     <row r="48" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="46"/>
       <c r="B48" s="47"/>
-      <c r="C48" s="97"/>
-      <c r="D48" s="98"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="77"/>
       <c r="E48" s="59"/>
       <c r="F48" s="60"/>
       <c r="G48" s="50"/>
@@ -3869,7 +3869,7 @@
       <c r="X48" s="53"/>
       <c r="Y48" s="53"/>
       <c r="Z48" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA48" s="53"/>
@@ -3881,8 +3881,8 @@
     <row r="49" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="46"/>
       <c r="B49" s="47"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="98"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="77"/>
       <c r="E49" s="59"/>
       <c r="F49" s="60"/>
       <c r="G49" s="50"/>
@@ -3905,7 +3905,7 @@
       <c r="X49" s="53"/>
       <c r="Y49" s="53"/>
       <c r="Z49" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA49" s="53"/>
@@ -3917,8 +3917,8 @@
     <row r="50" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="46"/>
       <c r="B50" s="47"/>
-      <c r="C50" s="97"/>
-      <c r="D50" s="98"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="77"/>
       <c r="E50" s="62"/>
       <c r="F50" s="63"/>
       <c r="G50" s="64"/>
@@ -3941,7 +3941,7 @@
       <c r="X50" s="53"/>
       <c r="Y50" s="53"/>
       <c r="Z50" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA50" s="53"/>
@@ -3953,8 +3953,8 @@
     <row r="51" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="46"/>
       <c r="B51" s="47"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="98"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="77"/>
       <c r="E51" s="66"/>
       <c r="F51" s="63"/>
       <c r="G51" s="67"/>
@@ -3977,7 +3977,7 @@
       <c r="X51" s="53"/>
       <c r="Y51" s="53"/>
       <c r="Z51" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA51" s="53"/>
@@ -3989,8 +3989,8 @@
     <row r="52" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="46"/>
       <c r="B52" s="47"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="98"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="77"/>
       <c r="E52" s="69"/>
       <c r="F52" s="70"/>
       <c r="G52" s="71"/>
@@ -4013,7 +4013,7 @@
       <c r="X52" s="53"/>
       <c r="Y52" s="53"/>
       <c r="Z52" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA52" s="53"/>
@@ -4025,8 +4025,8 @@
     <row r="53" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="46"/>
       <c r="B53" s="47"/>
-      <c r="C53" s="97"/>
-      <c r="D53" s="98"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="77"/>
       <c r="E53" s="69"/>
       <c r="F53" s="70"/>
       <c r="G53" s="72"/>
@@ -4049,7 +4049,7 @@
       <c r="X53" s="53"/>
       <c r="Y53" s="53"/>
       <c r="Z53" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA53" s="53"/>
@@ -4061,8 +4061,8 @@
     <row r="54" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="46"/>
       <c r="B54" s="47"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="98"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="77"/>
       <c r="E54" s="69"/>
       <c r="F54" s="73"/>
       <c r="G54" s="72"/>
@@ -4085,7 +4085,7 @@
       <c r="X54" s="53"/>
       <c r="Y54" s="53"/>
       <c r="Z54" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA54" s="53"/>
@@ -4097,8 +4097,8 @@
     <row r="55" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="46"/>
       <c r="B55" s="47"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="98"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="77"/>
       <c r="E55" s="69"/>
       <c r="F55" s="74"/>
       <c r="G55" s="72"/>
@@ -4121,7 +4121,7 @@
       <c r="X55" s="53"/>
       <c r="Y55" s="53"/>
       <c r="Z55" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA55" s="53"/>
@@ -4133,8 +4133,8 @@
     <row r="56" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="46"/>
       <c r="B56" s="47"/>
-      <c r="C56" s="97"/>
-      <c r="D56" s="98"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="77"/>
       <c r="E56" s="75"/>
       <c r="F56" s="74"/>
       <c r="G56" s="72"/>
@@ -4157,7 +4157,7 @@
       <c r="X56" s="53"/>
       <c r="Y56" s="53"/>
       <c r="Z56" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA56" s="53"/>
@@ -4169,8 +4169,8 @@
     <row r="57" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="46"/>
       <c r="B57" s="47"/>
-      <c r="C57" s="97"/>
-      <c r="D57" s="98"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="77"/>
       <c r="E57" s="69"/>
       <c r="F57" s="74"/>
       <c r="G57" s="72"/>
@@ -4193,7 +4193,7 @@
       <c r="X57" s="53"/>
       <c r="Y57" s="53"/>
       <c r="Z57" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA57" s="53"/>
@@ -4205,8 +4205,8 @@
     <row r="58" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="46"/>
       <c r="B58" s="47"/>
-      <c r="C58" s="97"/>
-      <c r="D58" s="98"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="77"/>
       <c r="E58" s="48"/>
       <c r="F58" s="49"/>
       <c r="G58" s="50"/>
@@ -4229,7 +4229,7 @@
       <c r="X58" s="53"/>
       <c r="Y58" s="53"/>
       <c r="Z58" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA58" s="53"/>
@@ -4241,8 +4241,8 @@
     <row r="59" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="46"/>
       <c r="B59" s="47"/>
-      <c r="C59" s="97"/>
-      <c r="D59" s="98"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="77"/>
       <c r="E59" s="59"/>
       <c r="F59" s="60"/>
       <c r="G59" s="50"/>
@@ -4265,7 +4265,7 @@
       <c r="X59" s="53"/>
       <c r="Y59" s="53"/>
       <c r="Z59" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA59" s="53"/>
@@ -4277,8 +4277,8 @@
     <row r="60" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="46"/>
       <c r="B60" s="47"/>
-      <c r="C60" s="97"/>
-      <c r="D60" s="98"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="77"/>
       <c r="E60" s="59"/>
       <c r="F60" s="60"/>
       <c r="G60" s="50"/>
@@ -4301,7 +4301,7 @@
       <c r="X60" s="53"/>
       <c r="Y60" s="53"/>
       <c r="Z60" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA60" s="53"/>
@@ -4313,8 +4313,8 @@
     <row r="61" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="46"/>
       <c r="B61" s="47"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="98"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="77"/>
       <c r="E61" s="62"/>
       <c r="F61" s="63"/>
       <c r="G61" s="64"/>
@@ -4337,7 +4337,7 @@
       <c r="X61" s="53"/>
       <c r="Y61" s="53"/>
       <c r="Z61" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA61" s="53"/>
@@ -4349,8 +4349,8 @@
     <row r="62" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="46"/>
       <c r="B62" s="47"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="98"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="77"/>
       <c r="E62" s="66"/>
       <c r="F62" s="63"/>
       <c r="G62" s="67"/>
@@ -4373,7 +4373,7 @@
       <c r="X62" s="53"/>
       <c r="Y62" s="53"/>
       <c r="Z62" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA62" s="53"/>
@@ -4385,8 +4385,8 @@
     <row r="63" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="46"/>
       <c r="B63" s="47"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="98"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="77"/>
       <c r="E63" s="69"/>
       <c r="F63" s="70"/>
       <c r="G63" s="71"/>
@@ -4409,7 +4409,7 @@
       <c r="X63" s="53"/>
       <c r="Y63" s="53"/>
       <c r="Z63" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA63" s="53"/>
@@ -4421,8 +4421,8 @@
     <row r="64" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="46"/>
       <c r="B64" s="47"/>
-      <c r="C64" s="97"/>
-      <c r="D64" s="98"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="77"/>
       <c r="E64" s="69"/>
       <c r="F64" s="70"/>
       <c r="G64" s="72"/>
@@ -4445,7 +4445,7 @@
       <c r="X64" s="53"/>
       <c r="Y64" s="53"/>
       <c r="Z64" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA64" s="53"/>
@@ -4457,8 +4457,8 @@
     <row r="65" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="46"/>
       <c r="B65" s="47"/>
-      <c r="C65" s="97"/>
-      <c r="D65" s="98"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="77"/>
       <c r="E65" s="69"/>
       <c r="F65" s="73"/>
       <c r="G65" s="72"/>
@@ -4481,7 +4481,7 @@
       <c r="X65" s="53"/>
       <c r="Y65" s="53"/>
       <c r="Z65" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA65" s="53"/>
@@ -4493,8 +4493,8 @@
     <row r="66" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="46"/>
       <c r="B66" s="47"/>
-      <c r="C66" s="97"/>
-      <c r="D66" s="98"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="77"/>
       <c r="E66" s="69"/>
       <c r="F66" s="74"/>
       <c r="G66" s="72"/>
@@ -4517,7 +4517,7 @@
       <c r="X66" s="53"/>
       <c r="Y66" s="53"/>
       <c r="Z66" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA66" s="53"/>
@@ -4529,8 +4529,8 @@
     <row r="67" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="46"/>
       <c r="B67" s="47"/>
-      <c r="C67" s="97"/>
-      <c r="D67" s="98"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="77"/>
       <c r="E67" s="75"/>
       <c r="F67" s="74"/>
       <c r="G67" s="72"/>
@@ -4553,7 +4553,7 @@
       <c r="X67" s="53"/>
       <c r="Y67" s="53"/>
       <c r="Z67" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA67" s="53"/>
@@ -4565,8 +4565,8 @@
     <row r="68" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="46"/>
       <c r="B68" s="47"/>
-      <c r="C68" s="97"/>
-      <c r="D68" s="98"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="77"/>
       <c r="E68" s="69"/>
       <c r="F68" s="74"/>
       <c r="G68" s="72"/>
@@ -4589,7 +4589,7 @@
       <c r="X68" s="53"/>
       <c r="Y68" s="53"/>
       <c r="Z68" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA68" s="53"/>
@@ -4601,8 +4601,8 @@
     <row r="69" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="46"/>
       <c r="B69" s="47"/>
-      <c r="C69" s="97"/>
-      <c r="D69" s="98"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="77"/>
       <c r="E69" s="48"/>
       <c r="F69" s="49"/>
       <c r="G69" s="50"/>
@@ -4625,7 +4625,7 @@
       <c r="X69" s="53"/>
       <c r="Y69" s="53"/>
       <c r="Z69" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA69" s="53"/>
@@ -4637,8 +4637,8 @@
     <row r="70" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="46"/>
       <c r="B70" s="47"/>
-      <c r="C70" s="97"/>
-      <c r="D70" s="98"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="77"/>
       <c r="E70" s="59"/>
       <c r="F70" s="60"/>
       <c r="G70" s="50"/>
@@ -4661,7 +4661,7 @@
       <c r="X70" s="53"/>
       <c r="Y70" s="53"/>
       <c r="Z70" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA70" s="53"/>
@@ -4673,8 +4673,8 @@
     <row r="71" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="46"/>
       <c r="B71" s="47"/>
-      <c r="C71" s="97"/>
-      <c r="D71" s="98"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="77"/>
       <c r="E71" s="59"/>
       <c r="F71" s="60"/>
       <c r="G71" s="50"/>
@@ -4697,7 +4697,7 @@
       <c r="X71" s="53"/>
       <c r="Y71" s="53"/>
       <c r="Z71" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA71" s="53"/>
@@ -4709,8 +4709,8 @@
     <row r="72" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="46"/>
       <c r="B72" s="47"/>
-      <c r="C72" s="97"/>
-      <c r="D72" s="98"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="77"/>
       <c r="E72" s="62"/>
       <c r="F72" s="63"/>
       <c r="G72" s="64"/>
@@ -4733,7 +4733,7 @@
       <c r="X72" s="53"/>
       <c r="Y72" s="53"/>
       <c r="Z72" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA72" s="53"/>
@@ -4745,8 +4745,8 @@
     <row r="73" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="46"/>
       <c r="B73" s="47"/>
-      <c r="C73" s="97"/>
-      <c r="D73" s="98"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="77"/>
       <c r="E73" s="66"/>
       <c r="F73" s="63"/>
       <c r="G73" s="67"/>
@@ -4769,7 +4769,7 @@
       <c r="X73" s="53"/>
       <c r="Y73" s="53"/>
       <c r="Z73" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA73" s="53"/>
@@ -4781,8 +4781,8 @@
     <row r="74" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="46"/>
       <c r="B74" s="47"/>
-      <c r="C74" s="97"/>
-      <c r="D74" s="98"/>
+      <c r="C74" s="76"/>
+      <c r="D74" s="77"/>
       <c r="E74" s="69"/>
       <c r="F74" s="70"/>
       <c r="G74" s="71"/>
@@ -4805,7 +4805,7 @@
       <c r="X74" s="53"/>
       <c r="Y74" s="53"/>
       <c r="Z74" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA74" s="53"/>
@@ -4817,8 +4817,8 @@
     <row r="75" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="46"/>
       <c r="B75" s="47"/>
-      <c r="C75" s="97"/>
-      <c r="D75" s="98"/>
+      <c r="C75" s="76"/>
+      <c r="D75" s="77"/>
       <c r="E75" s="69"/>
       <c r="F75" s="70"/>
       <c r="G75" s="72"/>
@@ -4841,7 +4841,7 @@
       <c r="X75" s="53"/>
       <c r="Y75" s="53"/>
       <c r="Z75" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA75" s="53"/>
@@ -4853,8 +4853,8 @@
     <row r="76" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="46"/>
       <c r="B76" s="47"/>
-      <c r="C76" s="97"/>
-      <c r="D76" s="98"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="77"/>
       <c r="E76" s="69"/>
       <c r="F76" s="73"/>
       <c r="G76" s="72"/>
@@ -4877,7 +4877,7 @@
       <c r="X76" s="53"/>
       <c r="Y76" s="53"/>
       <c r="Z76" s="57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA76" s="53"/>
@@ -4888,66 +4888,19 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="H1:N3"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="V6:Z6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="V7:Z7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="V8:Z8"/>
     <mergeCell ref="N13:U13"/>
     <mergeCell ref="V13:Z13"/>
     <mergeCell ref="H9:J9"/>
@@ -4961,19 +4914,66 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="K12:O12"/>
     <mergeCell ref="V12:Z12"/>
-    <mergeCell ref="V6:Z6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="V7:Z7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="V8:Z8"/>
-    <mergeCell ref="H1:N3"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
   </mergeCells>
   <conditionalFormatting sqref="M28:M35 M39:M46 M50:M57 M61:M68 M72:M76 K25:K30 K32:K76">
     <cfRule type="cellIs" dxfId="32" priority="32" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Changes made until 06/7/22 15:49 almost done with all test cases
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3bb12600baa2005/Documents/TRABAJO/TechMahindra/bootcamp/SampleProject_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="11_F25DC773A252ABDACC104880295A4B9C5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CFE355-5C5E-405A-9AC4-50410CC22866}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="11_F25DC773A252ABDACC104880295A4B9C5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD1B7215-7782-4296-8E85-627788844AE4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,9 +274,6 @@
     <t>AddingProducts</t>
   </si>
   <si>
-    <t xml:space="preserve">As a user I want to purchase a product stored on the cart </t>
-  </si>
-  <si>
     <t>As a user I want to delete items from the cart</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>DeletingProducts</t>
   </si>
   <si>
-    <t xml:space="preserve">User can purchase products added to the cart </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Load the website.                  2. Log in on the website.                            3. Click on cart.                                                                  4. Check number of products in the cart.              5. Click on the delete button.                             6. Confirm item has been deleted                                                      </t>
   </si>
   <si>
@@ -320,6 +314,12 @@
   </si>
   <si>
     <t xml:space="preserve">User can use contact form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I want to buy a product stored on the cart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can buy products added to the cart </t>
   </si>
 </sst>
 </file>
@@ -1826,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,7 +2038,7 @@
       <c r="J6" s="82"/>
       <c r="K6" s="96">
         <f>COUNTIF($Z$25:$Z$1000,"Ok")+COUNTIF($Z$25:$Z$1000,"FALLO")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L6" s="90"/>
       <c r="M6" s="90"/>
@@ -2075,7 +2075,7 @@
       <c r="J7" s="82"/>
       <c r="K7" s="96">
         <f>COUNTIF($Z$25:$Z$1000,"Ok")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L7" s="90"/>
       <c r="M7" s="90"/>
@@ -2149,7 +2149,7 @@
       <c r="J9" s="88"/>
       <c r="K9" s="89">
         <f>SUM(K5-K6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L9" s="90"/>
       <c r="M9" s="90"/>
@@ -2186,7 +2186,7 @@
       <c r="J10" s="82"/>
       <c r="K10" s="92">
         <f>($K$17+$L$17+$M$17+N$17+O$17)/($K$5)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L10" s="93"/>
       <c r="M10" s="93"/>
@@ -2225,7 +2225,7 @@
       <c r="J11" s="82"/>
       <c r="K11" s="92">
         <f>$K$6/($K$5)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L11" s="93"/>
       <c r="M11" s="93"/>
@@ -2264,7 +2264,7 @@
       <c r="J12" s="84"/>
       <c r="K12" s="92">
         <f>$K$7/($K$5)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L12" s="93"/>
       <c r="M12" s="93"/>
@@ -2462,7 +2462,7 @@
       <c r="J17" s="82"/>
       <c r="K17" s="31">
         <f>SUM(K18,K19)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L17" s="31">
         <f>SUM(L18,L19)</f>
@@ -2514,7 +2514,7 @@
       <c r="J18" s="82"/>
       <c r="K18" s="31">
         <f>COUNTIF($K$25:$K$1000,"Successful")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L18" s="31">
         <f>COUNTIF($N$25:$N$1000,"Exitoso")</f>
@@ -2618,7 +2618,7 @@
       <c r="J20" s="82"/>
       <c r="K20" s="32">
         <f>$K$17/($K$16)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L20" s="32">
         <f>$L$17/($L$16)</f>
@@ -2668,7 +2668,7 @@
       <c r="J21" s="84"/>
       <c r="K21" s="32">
         <f>$K$18/($K$16)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L21" s="32">
         <f>$L$18/($L$16)</f>
@@ -3014,11 +3014,11 @@
       <c r="A28" s="46"/>
       <c r="B28" s="47"/>
       <c r="C28" s="76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="77"/>
       <c r="E28" s="62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F28" s="60" t="s">
         <v>50</v>
@@ -3027,13 +3027,13 @@
         <v>4</v>
       </c>
       <c r="H28" s="51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I28" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J28" s="53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K28" s="54" t="s">
         <v>39</v>
@@ -3192,7 +3192,7 @@
         <v>70</v>
       </c>
       <c r="K31" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L31" s="65"/>
       <c r="M31" s="56"/>
@@ -3210,7 +3210,7 @@
       <c r="Y31" s="53"/>
       <c r="Z31" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>PENDING</v>
+        <v>OK</v>
       </c>
       <c r="AA31" s="53"/>
       <c r="AB31" s="58"/>
@@ -3244,7 +3244,7 @@
         <v>75</v>
       </c>
       <c r="K32" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L32" s="65"/>
       <c r="M32" s="56"/>
@@ -3262,7 +3262,7 @@
       <c r="Y32" s="53"/>
       <c r="Z32" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>PENDING</v>
+        <v>OK</v>
       </c>
       <c r="AA32" s="53"/>
       <c r="AB32" s="58"/>
@@ -3274,29 +3274,29 @@
       <c r="A33" s="46"/>
       <c r="B33" s="47"/>
       <c r="C33" s="76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="77"/>
       <c r="E33" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="60" t="s">
         <v>78</v>
-      </c>
-      <c r="F33" s="60" t="s">
-        <v>79</v>
       </c>
       <c r="G33" s="72">
         <v>9</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I33" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="J33" s="53" t="s">
-        <v>81</v>
-      </c>
       <c r="K33" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L33" s="65"/>
       <c r="M33" s="56"/>
@@ -3314,7 +3314,7 @@
       <c r="Y33" s="53"/>
       <c r="Z33" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>PENDING</v>
+        <v>OK</v>
       </c>
       <c r="AA33" s="53"/>
       <c r="AB33" s="58"/>
@@ -3326,29 +3326,29 @@
       <c r="A34" s="46"/>
       <c r="B34" s="47"/>
       <c r="C34" s="76" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D34" s="77"/>
       <c r="E34" s="75" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F34" s="60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G34" s="72">
         <v>10</v>
       </c>
       <c r="H34" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="I34" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="J34" s="53" t="s">
-        <v>86</v>
-      </c>
       <c r="K34" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L34" s="65"/>
       <c r="M34" s="56"/>
@@ -3366,7 +3366,7 @@
       <c r="Y34" s="53"/>
       <c r="Z34" s="57" t="str">
         <f t="shared" si="0"/>
-        <v>PENDING</v>
+        <v>OK</v>
       </c>
       <c r="AA34" s="53"/>
       <c r="AB34" s="58"/>
@@ -3509,7 +3509,7 @@
       <c r="X38" s="53"/>
       <c r="Y38" s="53"/>
       <c r="Z38" s="57" t="b">
-        <f t="shared" ref="Z26:Z76" si="1">IF(W38="Exitoso","OK",IF(W38="Fallido","FALLO",IF(W38="Pendiente","PENDIENTE",IF(T38="Exitoso","OK",IF(T38="Fallido","FALLO",IF(T38="Pendiente","PENDIENTE",IF(Q38="Exitoso","OK",IF(Q38="Fallido","FALLO",IF(Q38="Pendiente","PENDIENTE",IF(N38="Exitoso","OK",IF(N38="Fallido","FALLO",IF(N38="Pendiente","PENDIENTE",IF(K38="Exitoso","OK",IF(K38="Fallido","FALLO",IF(K38="Pendiente","PENDIENTE")))))))))))))))</f>
+        <f t="shared" ref="Z38:Z76" si="1">IF(W38="Exitoso","OK",IF(W38="Fallido","FALLO",IF(W38="Pendiente","PENDIENTE",IF(T38="Exitoso","OK",IF(T38="Fallido","FALLO",IF(T38="Pendiente","PENDIENTE",IF(Q38="Exitoso","OK",IF(Q38="Fallido","FALLO",IF(Q38="Pendiente","PENDIENTE",IF(N38="Exitoso","OK",IF(N38="Fallido","FALLO",IF(N38="Pendiente","PENDIENTE",IF(K38="Exitoso","OK",IF(K38="Fallido","FALLO",IF(K38="Pendiente","PENDIENTE")))))))))))))))</f>
         <v>0</v>
       </c>
       <c r="AA38" s="53"/>

</xml_diff>